<commit_message>
committed with stale element issue
</commit_message>
<xml_diff>
--- a/target/classes/testdata/OPAS_TestData.xlsx
+++ b/target/classes/testdata/OPAS_TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanpr\exlipsefolder2\DFAT_APO\src\test\java\dfat\apo\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanpr\exlipsefolder2\DFAT_PassportProject\src\main\java\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD1177BD-B63F-4A10-99D1-D8F1FF079851}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A6F833B-CBB5-4B73-9574-31B0CEC01998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{84FAEEE2-7639-48EA-AA82-76271FAE16F1}"/>
+    <workbookView xWindow="32880" yWindow="6090" windowWidth="21600" windowHeight="11295" xr2:uid="{84FAEEE2-7639-48EA-AA82-76271FAE16F1}"/>
   </bookViews>
   <sheets>
     <sheet name="OPAS_SIT" sheetId="1" r:id="rId1"/>
@@ -551,13 +551,13 @@
   <dimension ref="A1:AE3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.28515625" customWidth="1"/>
     <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>

</xml_diff>